<commit_message>
ServiceRequest (Order Details for Diag Rep) - drafted for DR
Generation of output
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-02:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-03:The requester of the diagnostic investigation order shall be a PractitionerRole {basedOn.resolve().requester.resolve().where($this is PractitionerRole).exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}inv-dh-dir-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-dir-02:The performer shall at least have a reference or an identifier with at least a system and a value {performer.reference.exists() or performer.identifier.where(system.count() + value.count() &gt;1).exists()}</t>
   </si>
   <si>
     <t>Event</t>
@@ -561,7 +561,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/servicerequest-otherdiag-report-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/servicerequest-diag-report-1)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Regerated outputs from the changes to My Health Record Other Diagnostic Report
- DiagnsoticReport.presentedForm cardinality changed from 1..1 to 0..*
- Removed the fixed value application/pdf
- Added implementation guidance on providing attachments

DR-193
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="433">
   <si>
     <t>Path</t>
   </si>
@@ -1194,9 +1194,6 @@
   </si>
   <si>
     <t>Processors of the data need to be able to know how to interpret the data.</t>
-  </si>
-  <si>
-    <t>application/pdf</t>
   </si>
   <si>
     <t>text/plain; charset=UTF-8, image/png</t>
@@ -7366,10 +7363,10 @@
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>53</v>
@@ -7731,13 +7728,13 @@
       </c>
       <c r="P56" s="2"/>
       <c r="Q56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="R56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="S56" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="R56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S56" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="T56" t="s" s="2">
         <v>43</v>
@@ -7752,28 +7749,28 @@
         <v>212</v>
       </c>
       <c r="X56" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="Y56" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="Y56" t="s" s="2">
+      <c r="Z56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE56" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7791,10 +7788,10 @@
         <v>43</v>
       </c>
       <c r="AK56" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AL56" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>43</v>
@@ -7802,7 +7799,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7828,14 +7825,14 @@
         <v>129</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>43</v>
@@ -7884,7 +7881,7 @@
         <v>43</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7905,7 +7902,7 @@
         <v>43</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>43</v>
@@ -7913,7 +7910,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7936,19 +7933,19 @@
         <v>43</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="K58" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="K58" t="s" s="2">
+      <c r="L58" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>43</v>
@@ -7997,7 +7994,7 @@
         <v>43</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -8015,10 +8012,10 @@
         <v>43</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="AL58" t="s" s="2">
         <v>394</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>43</v>
@@ -8026,7 +8023,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8049,19 +8046,19 @@
         <v>53</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>43</v>
@@ -8074,43 +8071,43 @@
         <v>43</v>
       </c>
       <c r="S59" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="T59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD59" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE59" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="T59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE59" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8128,10 +8125,10 @@
         <v>43</v>
       </c>
       <c r="AK59" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AL59" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>405</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>43</v>
@@ -8139,7 +8136,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8162,19 +8159,19 @@
         <v>53</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>411</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>43</v>
@@ -8223,7 +8220,7 @@
         <v>43</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8244,7 +8241,7 @@
         <v>43</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>43</v>
@@ -8252,7 +8249,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8275,19 +8272,19 @@
         <v>53</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>43</v>
@@ -8336,7 +8333,7 @@
         <v>43</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8357,7 +8354,7 @@
         <v>43</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>43</v>
@@ -8365,7 +8362,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8391,14 +8388,14 @@
         <v>54</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>43</v>
@@ -8411,43 +8408,43 @@
         <v>43</v>
       </c>
       <c r="S62" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="T62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="U62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="V62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="W62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="X62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Y62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="Z62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AA62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AB62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AC62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AD62" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AE62" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>426</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8468,7 +8465,7 @@
         <v>43</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>43</v>
@@ -8476,7 +8473,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8499,17 +8496,17 @@
         <v>53</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O63" t="s" s="2">
         <v>43</v>
@@ -8558,7 +8555,7 @@
         <v>43</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>41</v>
@@ -8579,7 +8576,7 @@
         <v>43</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
Regenerated the outputs after the changes for My Health Record Other Diagnostic Report "presentedForm" element
DR-193
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
+++ b/output/DiagnosticReport/diagnosticreport-otherdiag-mhr-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AM$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="368">
   <si>
     <t>Path</t>
   </si>
@@ -1176,205 +1176,6 @@
   </si>
   <si>
     <t>text (type=ED)</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.id</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.extension</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.contentType</t>
-  </si>
-  <si>
-    <t>Mime type of the content, with charset etc.</t>
-  </si>
-  <si>
-    <t>Identifies the type of the data in the attachment and allows a method to be chosen to interpret or render the data. Includes mime type parameters such as charset where appropriate.</t>
-  </si>
-  <si>
-    <t>Processors of the data need to be able to know how to interpret the data.</t>
-  </si>
-  <si>
-    <t>text/plain; charset=UTF-8, image/png</t>
-  </si>
-  <si>
-    <t>The mime type of an attachment. Any valid mime type is allowed.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/mimetypes|4.0.1</t>
-  </si>
-  <si>
-    <t>Attachment.contentType</t>
-  </si>
-  <si>
-    <t>ED.2+ED.3/RP.2+RP.3. Note conversion may be needed if old style values are being used</t>
-  </si>
-  <si>
-    <t>./mediaType, ./charset</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.language</t>
-  </si>
-  <si>
-    <t>Human language of the content (BCP-47)</t>
-  </si>
-  <si>
-    <t>The human language of the content. The value can be any valid value according to BCP 47.</t>
-  </si>
-  <si>
-    <t>Users need to be able to choose between the languages in a set of attachments.</t>
-  </si>
-  <si>
-    <t>Attachment.language</t>
-  </si>
-  <si>
-    <t>./language</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base64Binary
-</t>
-  </si>
-  <si>
-    <t>Data inline, base64ed</t>
-  </si>
-  <si>
-    <t>The actual data of the attachment - a sequence of bytes, base64 encoded.</t>
-  </si>
-  <si>
-    <t>The base64-encoded data SHALL be expressed in the same character set as the base resource XML or JSON.</t>
-  </si>
-  <si>
-    <t>The data needs to able to be transmitted inline.</t>
-  </si>
-  <si>
-    <t>Attachment.data</t>
-  </si>
-  <si>
-    <t>ED.5</t>
-  </si>
-  <si>
-    <t>./data</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url
-</t>
-  </si>
-  <si>
-    <t>Uri where the data can be found</t>
-  </si>
-  <si>
-    <t>A location where the data can be accessed.</t>
-  </si>
-  <si>
-    <t>If both data and url are provided, the url SHALL point to the same content as the data contains. Urls may be relative references or may reference transient locations such as a wrapping envelope using cid: though this has ramifications for using signatures. Relative URLs are interpreted relative to the service url, like a resource reference, rather than relative to the resource itself. If a URL is provided, it SHALL resolve to actual data.</t>
-  </si>
-  <si>
-    <t>The data needs to be transmitted by reference.</t>
-  </si>
-  <si>
-    <t>http://www.acme.com/logo-small.png</t>
-  </si>
-  <si>
-    <t>Attachment.url</t>
-  </si>
-  <si>
-    <t>RP.1+RP.2 - if they refer to a URL (see v2.6)</t>
-  </si>
-  <si>
-    <t>./reference/literal</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unsignedInt
-</t>
-  </si>
-  <si>
-    <t>Number of bytes of content (if url provided)</t>
-  </si>
-  <si>
-    <t>The number of bytes of data that make up this attachment (before base64 encoding, if that is done).</t>
-  </si>
-  <si>
-    <t>The number of bytes is redundant if the data is provided as a base64binary, but is useful if the data is provided as a url reference.</t>
-  </si>
-  <si>
-    <t>Representing the size allows applications to determine whether they should fetch the content automatically in advance, or refuse to fetch it at all.</t>
-  </si>
-  <si>
-    <t>Attachment.size</t>
-  </si>
-  <si>
-    <t>N/A (needs data type R3 proposal)</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.hash</t>
-  </si>
-  <si>
-    <t>Hash of the data (sha-1, base64ed)</t>
-  </si>
-  <si>
-    <t>The calculated hash of the data using SHA-1. Represented using base64.</t>
-  </si>
-  <si>
-    <t>The hash is calculated on the data prior to base64 encoding, if the data is based64 encoded. The hash is not intended to support digital signatures. Where protection against malicious threats a digital signature should be considered, see [Provenance.signature](http://hl7.org/fhir/R4/provenance-definitions.html#Provenance.signature) for mechanism to protect a resource with a digital signature.</t>
-  </si>
-  <si>
-    <t>Included so that applications can verify that the contents of a location have not changed due to technical failures (e.g., storage rot, transport glitch, incorrect version).</t>
-  </si>
-  <si>
-    <t>Attachment.hash</t>
-  </si>
-  <si>
-    <t>.integrityCheck[parent::ED/integrityCheckAlgorithm="SHA-1"]</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.title</t>
-  </si>
-  <si>
-    <t>Label to display in place of the data</t>
-  </si>
-  <si>
-    <t>A label or set of text to display in place of the data.</t>
-  </si>
-  <si>
-    <t>Applications need a label to display to a human user in place of the actual data if the data cannot be rendered or perceived by the viewer.</t>
-  </si>
-  <si>
-    <t>Official Corporate Logo</t>
-  </si>
-  <si>
-    <t>Attachment.title</t>
-  </si>
-  <si>
-    <t>./title/data</t>
-  </si>
-  <si>
-    <t>DiagnosticReport.presentedForm.creation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateTime
-</t>
-  </si>
-  <si>
-    <t>Date attachment was first created</t>
-  </si>
-  <si>
-    <t>The date that the attachment was first created.</t>
-  </si>
-  <si>
-    <t>This is often tracked as an integrity issue for use of the attachment.</t>
-  </si>
-  <si>
-    <t>Attachment.creation</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1324,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM63"/>
+  <dimension ref="A1:AM53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1532,7 +1333,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="42.65234375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="39.4296875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="60.54296875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -7466,1124 +7267,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" hidden="true">
-      <c r="A55" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F55" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="N55" s="2"/>
-      <c r="O55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="56" hidden="true">
-      <c r="A56" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F56" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I56" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J56" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="K56" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="M56" s="2"/>
-      <c r="N56" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="O56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P56" s="2"/>
-      <c r="Q56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S56" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="T56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W56" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="X56" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="Y56" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" hidden="true">
-      <c r="A57" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F57" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I57" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J57" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="K57" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="M57" s="2"/>
-      <c r="N57" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="O57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P57" s="2"/>
-      <c r="Q57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S57" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="T57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W57" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="X57" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="Y57" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="Z57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE57" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="AF57" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG57" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI57" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" hidden="true">
-      <c r="A58" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F58" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="J58" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="K58" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="O58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P58" s="2"/>
-      <c r="Q58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE58" t="s" s="2">
-        <v>392</v>
-      </c>
-      <c r="AF58" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG58" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI58" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ58" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>393</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" hidden="true">
-      <c r="A59" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F59" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I59" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J59" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="K59" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="O59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P59" s="2"/>
-      <c r="Q59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S59" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="T59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE59" t="s" s="2">
-        <v>402</v>
-      </c>
-      <c r="AF59" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG59" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI59" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ59" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK59" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60" hidden="true">
-      <c r="A60" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="B60" s="2"/>
-      <c r="C60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F60" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I60" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J60" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="K60" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="O60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P60" s="2"/>
-      <c r="Q60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE60" t="s" s="2">
-        <v>411</v>
-      </c>
-      <c r="AF60" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" hidden="true">
-      <c r="A61" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F61" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I61" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J61" t="s" s="2">
-        <v>387</v>
-      </c>
-      <c r="K61" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="O61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P61" s="2"/>
-      <c r="Q61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" hidden="true">
-      <c r="A62" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="F62" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I62" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J62" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="M62" s="2"/>
-      <c r="N62" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="O62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P62" s="2"/>
-      <c r="Q62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S62" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="AF62" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG62" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI62" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="63" hidden="true">
-      <c r="A63" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F63" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="G63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="H63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="I63" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="J63" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="K63" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="M63" s="2"/>
-      <c r="N63" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="O63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="P63" s="2"/>
-      <c r="Q63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="R63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="S63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="T63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="U63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="V63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="W63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="X63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Y63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="AF63" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG63" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="AH63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AI63" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AJ63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AM63">
+  <autoFilter ref="A1:AM53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8593,7 +7278,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI62">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>